<commit_message>
results of the 200RFQ experiments are added
</commit_message>
<xml_diff>
--- a/analysis_line_chart(AutoRecovered).xlsx
+++ b/analysis_line_chart(AutoRecovered).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vodel\VODELYA\PhD\SmartChainDB\smartchaindb-experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nodir\OneDrive\Desktop\final_experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0641B487-4988-497F-A688-3A635C9537ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7623DF0D-883A-4732-B668-12FAD7EC4CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9636" yWindow="954" windowWidth="11154" windowHeight="10542" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2805" yWindow="1620" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAPs" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="17">
   <si>
     <t>Capabilities</t>
   </si>
@@ -66,6 +66,18 @@
   </si>
   <si>
     <t>SCDB</t>
+  </si>
+  <si>
+    <t>Labels</t>
+  </si>
+  <si>
+    <t>20-25</t>
+  </si>
+  <si>
+    <t>100-25</t>
+  </si>
+  <si>
+    <t>200-25</t>
   </si>
 </sst>
 </file>
@@ -198,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -221,6 +233,9 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -236,9 +251,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -252,6 +264,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5465,7 +5480,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'tx-num'!$A$4</c:f>
+              <c:f>'tx-num'!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5544,7 +5559,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'tx-num'!$B$3:$E$3</c:f>
+              <c:f>'tx-num'!$C$3:$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -5564,7 +5579,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tx-num'!$B$4:$E$4</c:f>
+              <c:f>'tx-num'!$C$4:$F$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -5594,7 +5609,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'tx-num'!$A$12</c:f>
+              <c:f>'tx-num'!$B$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5673,7 +5688,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'tx-num'!$B$3:$E$3</c:f>
+              <c:f>'tx-num'!$C$3:$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -5693,7 +5708,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tx-num'!$C$12:$F$12</c:f>
+              <c:f>'tx-num'!$D$12:$G$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -6116,7 +6131,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'tx-num'!$A$5</c:f>
+              <c:f>'tx-num'!$B$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6195,7 +6210,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'tx-num'!$C$11:$F$11</c:f>
+              <c:f>'tx-num'!$D$11:$G$11</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -6215,7 +6230,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tx-num'!$B$5:$E$5</c:f>
+              <c:f>'tx-num'!$C$5:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -6245,7 +6260,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'tx-num'!$A$13</c:f>
+              <c:f>'tx-num'!$B$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6324,7 +6339,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'tx-num'!$C$11:$F$11</c:f>
+              <c:f>'tx-num'!$D$11:$G$11</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -6344,7 +6359,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tx-num'!$C$13:$F$13</c:f>
+              <c:f>'tx-num'!$D$13:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -11273,13 +11288,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>241253</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>7797</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>577430</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>77273</xdr:rowOff>
@@ -11309,16 +11324,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>188810</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>103085</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>127617</xdr:rowOff>
+      <xdr:rowOff>89517</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>492145</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>13317</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>406420</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>165717</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11617,28 +11632,28 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.15625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="13"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -11655,7 +11670,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>15</v>
       </c>
@@ -11672,7 +11687,7 @@
         <v>1243.5999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>30</v>
       </c>
@@ -11689,7 +11704,7 @@
         <v>1317.65</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45</v>
       </c>
@@ -11706,7 +11721,7 @@
         <v>1378.6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>60</v>
       </c>
@@ -11723,27 +11738,27 @@
         <v>1332.3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="13"/>
+      <c r="B9" s="14"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -11763,7 +11778,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>15</v>
       </c>
@@ -11783,7 +11798,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>30</v>
       </c>
@@ -11803,7 +11818,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45</v>
       </c>
@@ -11823,7 +11838,7 @@
         <v>4679</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>60</v>
       </c>
@@ -11858,207 +11873,234 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E4E959-0883-4ECC-862F-8D76850309AF}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="B1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F21" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="C1" s="23"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="7"/>
-      <c r="B2" s="18" t="s">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="7"/>
+      <c r="C2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="19"/>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="D3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="11">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="11">
         <v>1317.65</v>
       </c>
-      <c r="C4" s="11">
+      <c r="D4" s="11">
         <v>10286.07</v>
       </c>
-      <c r="D4" s="11">
+      <c r="E4" s="11">
         <v>243.3</v>
       </c>
-      <c r="E4" s="11">
+      <c r="F4" s="11">
         <v>217.01400000000001</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="11">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="11">
         <v>1468.95</v>
       </c>
-      <c r="C5" s="11">
+      <c r="D5" s="11">
         <v>10992.1468</v>
       </c>
-      <c r="D5" s="11">
+      <c r="E5" s="11">
         <v>250.29</v>
       </c>
-      <c r="E5" s="11">
+      <c r="F5" s="11">
         <v>231.30840000000001</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="8"/>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="8"/>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1"/>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="21" t="s">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="7"/>
-      <c r="B10" s="18" t="s">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="19"/>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
-      <c r="F10" s="20"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="C11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="E11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="F11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="11">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="11">
         <v>1479.89</v>
       </c>
-      <c r="C12" s="11">
+      <c r="D12" s="11">
         <v>1544</v>
       </c>
-      <c r="D12" s="11">
+      <c r="E12" s="11">
         <v>204.69</v>
       </c>
-      <c r="E12" s="11">
+      <c r="F12" s="11">
         <v>588.4</v>
       </c>
-      <c r="F12" s="11">
+      <c r="G12" s="11">
         <v>183.92</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="11">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="11">
         <v>6603.76</v>
       </c>
-      <c r="C13" s="11">
+      <c r="D13" s="11">
         <v>6772</v>
       </c>
-      <c r="D13" s="11">
+      <c r="E13" s="11">
         <v>217.66</v>
       </c>
-      <c r="E13" s="11">
+      <c r="F13" s="11">
         <v>573.75</v>
       </c>
-      <c r="F13" s="11">
+      <c r="G13" s="11">
         <v>79.3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="8">
+        <v>8082.22</v>
+      </c>
+      <c r="D14" s="8">
+        <v>8278</v>
+      </c>
+      <c r="E14" s="8">
+        <v>583.62</v>
+      </c>
+      <c r="F14" s="8">
+        <v>3132.94</v>
+      </c>
+      <c r="G14" s="8">
+        <v>189.18</v>
+      </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="8"/>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12074,15 +12116,15 @@
       <selection activeCell="G18" sqref="A1:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="23"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="18" t="s">
         <v>9</v>
@@ -12092,7 +12134,7 @@
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -12112,7 +12154,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>15</v>
       </c>
@@ -12122,7 +12164,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>30</v>
       </c>
@@ -12132,7 +12174,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>45</v>
       </c>
@@ -12142,7 +12184,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>60</v>
       </c>
@@ -12152,17 +12194,17 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="22"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="18" t="s">
         <v>9</v>
@@ -12172,7 +12214,7 @@
       <c r="E10" s="19"/>
       <c r="F10" s="20"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>0</v>
       </c>
@@ -12192,7 +12234,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>15</v>
       </c>
@@ -12212,7 +12254,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>30</v>
       </c>
@@ -12232,7 +12274,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>45</v>
       </c>
@@ -12252,7 +12294,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
fixed the analysis code
</commit_message>
<xml_diff>
--- a/analysis_line_chart(AutoRecovered).xlsx
+++ b/analysis_line_chart(AutoRecovered).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vodel\VODELYA\PhD\SmartChainDB\smartchaindb-experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nodir\OneDrive\Desktop\final_experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C067DF53-A193-4321-AE54-57689722897B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16483C44-1292-4BCB-82F3-F45F68EBE503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="408" yWindow="1422" windowWidth="17718" windowHeight="10542" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3930" yWindow="2415" windowWidth="21330" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAPs" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="17">
   <si>
     <t>Capabilities</t>
   </si>
@@ -210,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -268,6 +268,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5468,7 +5481,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18960884585381554"/>
+          <c:y val="0.17677589717578379"/>
+          <c:w val="0.75235202330810624"/>
+          <c:h val="0.50852190920000762"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
@@ -5722,21 +5745,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tx-num'!$D$12:$G$12</c:f>
+              <c:f>'tx-num'!$C$12:$F$12</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1544</c:v>
+                  <c:v>274.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>204.69</c:v>
+                  <c:v>91.66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>588.4</c:v>
+                  <c:v>263.95</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>183.92</c:v>
+                  <c:v>75.41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6247,7 +6270,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'tx-num'!$D$11:$G$11</c:f>
+              <c:f>'tx-num'!$C$11:$F$11</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -6373,7 +6396,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'tx-num'!$D$11:$G$11</c:f>
+              <c:f>'tx-num'!$C$11:$F$11</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -6393,21 +6416,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tx-num'!$D$13:$G$13</c:f>
+              <c:f>'tx-num'!$C$13:$F$13</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6772</c:v>
+                  <c:v>344.57</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>217.66</c:v>
+                  <c:v>98.88</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>573.75</c:v>
+                  <c:v>245.47</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>79.3</c:v>
+                  <c:v>81.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6900,7 +6923,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'tx-num'!$D$11:$G$11</c:f>
+              <c:f>'tx-num'!$C$11:$F$11</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -7026,7 +7049,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'tx-num'!$D$11:$G$11</c:f>
+              <c:f>'tx-num'!$C$11:$F$11</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -7046,21 +7069,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'tx-num'!$D$14:$G$14</c:f>
+              <c:f>'tx-num'!$C$14:$F$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8278</c:v>
+                  <c:v>386.98</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>583.62</c:v>
+                  <c:v>135.62</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3132.94</c:v>
+                  <c:v>241.32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>189.18</c:v>
+                  <c:v>82.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12908,19 +12931,19 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.15625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="13"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="15" t="s">
         <v>1</v>
@@ -12929,7 +12952,7 @@
       <c r="D2" s="16"/>
       <c r="E2" s="17"/>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -12946,7 +12969,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>15</v>
       </c>
@@ -12963,7 +12986,7 @@
         <v>1243.5999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>30</v>
       </c>
@@ -12980,7 +13003,7 @@
         <v>1317.65</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45</v>
       </c>
@@ -12997,7 +13020,7 @@
         <v>1378.6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>60</v>
       </c>
@@ -13014,17 +13037,17 @@
         <v>1332.3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="14"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="15" t="s">
         <v>1</v>
@@ -13034,7 +13057,7 @@
       <c r="E10" s="16"/>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -13054,7 +13077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>15</v>
       </c>
@@ -13074,7 +13097,7 @@
         <v>1313</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>30</v>
       </c>
@@ -13094,7 +13117,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45</v>
       </c>
@@ -13114,7 +13137,7 @@
         <v>4679</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>60</v>
       </c>
@@ -13151,32 +13174,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E4E959-0883-4ECC-862F-8D76850309AF}">
   <dimension ref="B1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="23" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="23"/>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="7"/>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="24"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
@@ -13192,11 +13215,8 @@
       <c r="F3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
@@ -13212,9 +13232,8 @@
       <c r="F4" s="11">
         <v>217.01400000000001</v>
       </c>
-      <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>15</v>
       </c>
@@ -13230,9 +13249,8 @@
       <c r="F5" s="11">
         <v>231.30840000000001</v>
       </c>
-      <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>16</v>
       </c>
@@ -13248,145 +13266,131 @@
       <c r="F6" s="8">
         <v>246.8314</v>
       </c>
-      <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="22"/>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="20"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="27"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="F11" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="11">
-        <v>1479.89</v>
-      </c>
-      <c r="D12" s="11">
-        <v>1544</v>
-      </c>
-      <c r="E12" s="11">
-        <v>204.69</v>
-      </c>
-      <c r="F12" s="11">
-        <v>588.4</v>
-      </c>
-      <c r="G12" s="11">
-        <v>183.92</v>
+      <c r="C12" s="28">
+        <v>274.8</v>
+      </c>
+      <c r="D12" s="28">
+        <v>91.66</v>
+      </c>
+      <c r="E12" s="28">
+        <v>263.95</v>
+      </c>
+      <c r="F12" s="28">
+        <v>75.41</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="11">
-        <v>6603.76</v>
-      </c>
-      <c r="D13" s="11">
-        <v>6772</v>
-      </c>
-      <c r="E13" s="11">
-        <v>217.66</v>
-      </c>
-      <c r="F13" s="11">
-        <v>573.75</v>
-      </c>
-      <c r="G13" s="11">
-        <v>79.3</v>
+      <c r="C13" s="28">
+        <v>344.57</v>
+      </c>
+      <c r="D13" s="28">
+        <v>98.88</v>
+      </c>
+      <c r="E13" s="28">
+        <v>245.47</v>
+      </c>
+      <c r="F13" s="28">
+        <v>81.8</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="8">
-        <v>8082.22</v>
-      </c>
-      <c r="D14" s="8">
-        <v>8278</v>
-      </c>
-      <c r="E14" s="8">
-        <v>583.62</v>
-      </c>
-      <c r="F14" s="8">
-        <v>3132.94</v>
-      </c>
-      <c r="G14" s="8">
-        <v>189.18</v>
+      <c r="C14" s="28">
+        <v>386.98</v>
+      </c>
+      <c r="D14" s="28">
+        <v>135.62</v>
+      </c>
+      <c r="E14" s="28">
+        <v>241.32</v>
+      </c>
+      <c r="F14" s="28">
+        <v>82.2</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="G15" s="26"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C10:G10"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="C2:G2"/>
     <mergeCell ref="B1:C1"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13402,15 +13406,15 @@
       <selection activeCell="G18" sqref="A1:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="23"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="18" t="s">
         <v>9</v>
@@ -13420,7 +13424,7 @@
       <c r="E2" s="19"/>
       <c r="F2" s="20"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -13440,7 +13444,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>15</v>
       </c>
@@ -13450,7 +13454,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>30</v>
       </c>
@@ -13460,7 +13464,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>45</v>
       </c>
@@ -13470,7 +13474,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>60</v>
       </c>
@@ -13480,17 +13484,17 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="22"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="18" t="s">
         <v>9</v>
@@ -13500,7 +13504,7 @@
       <c r="E10" s="19"/>
       <c r="F10" s="20"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>0</v>
       </c>
@@ -13520,7 +13524,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>15</v>
       </c>
@@ -13540,7 +13544,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>30</v>
       </c>
@@ -13560,7 +13564,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>45</v>
       </c>
@@ -13580,7 +13584,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>60</v>
       </c>

</xml_diff>